<commit_message>
chore: adjust audio playback timing and remove Russian audio button
</commit_message>
<xml_diff>
--- a/public/dictionaries/List7.xlsx
+++ b/public/dictionaries/List7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\FlashCards\public\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6B3C6-E48C-4087-87A9-8B42DAE871C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0292A61-C07B-4705-95D9-8A764D22BF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист7" sheetId="1" r:id="rId1"/>
@@ -412,12 +412,6 @@
     <t>statue</t>
   </si>
   <si>
-    <t>веселый</t>
-  </si>
-  <si>
-    <t>exiting</t>
-  </si>
-  <si>
     <t>синагога</t>
   </si>
   <si>
@@ -674,13 +668,20 @@
   </si>
   <si>
     <t>Effort</t>
+  </si>
+  <si>
+    <t>exciting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+захватывающий</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -705,6 +706,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -733,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -753,6 +762,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,8 +986,8 @@
   </sheetPr>
   <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1006,16 +1018,16 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1032,16 +1044,16 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="O2" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1058,16 +1070,16 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="O3" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1084,16 +1096,16 @@
         <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="O4" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1110,16 +1122,16 @@
         <v>19</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="O5" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1136,16 +1148,16 @@
         <v>23</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="O6" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1162,16 +1174,16 @@
         <v>27</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1188,16 +1200,16 @@
         <v>31</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="O8" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1214,16 +1226,16 @@
         <v>35</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="O9" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1240,16 +1252,16 @@
         <v>39</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="O10" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,16 +1278,16 @@
         <v>43</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="O11" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1292,16 +1304,16 @@
         <v>47</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="O12" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1318,16 +1330,16 @@
         <v>51</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1344,16 +1356,16 @@
         <v>55</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="O14" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1370,16 +1382,16 @@
         <v>59</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="O15" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1396,16 +1408,16 @@
         <v>63</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="O16" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1418,16 +1430,16 @@
       <c r="E17" s="5"/>
       <c r="G17" s="6"/>
       <c r="I17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="O17" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1436,16 +1448,16 @@
       <c r="E18" s="5"/>
       <c r="G18" s="6"/>
       <c r="I18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="O18" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,10 +1466,10 @@
       <c r="E19" s="5"/>
       <c r="G19" s="6"/>
       <c r="I19" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M19" s="5"/>
       <c r="O19" s="6"/>
@@ -1693,63 +1705,63 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="G38" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E40" s="5"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E41" s="5"/>
       <c r="G41" s="6"/>
@@ -7421,5 +7433,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: refactor word handling to use unique identifiers and update translation logic
</commit_message>
<xml_diff>
--- a/public/dictionaries/List7.xlsx
+++ b/public/dictionaries/List7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\FlashCards\public\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0292A61-C07B-4705-95D9-8A764D22BF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50C9108-75ED-4942-A320-7EB84CC71142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32475" yWindow="2100" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист7" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="221">
   <si>
     <t>Крупный план</t>
   </si>
@@ -675,13 +675,22 @@
   <si>
     <t xml:space="preserve">
 захватывающий</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Ukrainian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -715,6 +724,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -742,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -766,6 +784,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -984,10 +1003,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O1001"/>
+  <dimension ref="A1:O1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1005,459 +1024,467 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>147</v>
+      <c r="A1" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="I17" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="C18" s="8"/>
       <c r="E18" s="5"/>
       <c r="G18" s="6"/>
       <c r="I18" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1466,319 +1493,336 @@
       <c r="E19" s="5"/>
       <c r="G19" s="6"/>
       <c r="I19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="I20" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="M20" s="5"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="E27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="C28" s="8"/>
       <c r="E28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="E29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E41" s="5"/>
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="C42" s="8"/>
+      <c r="A42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="G42" s="6"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="7"/>
       <c r="C43" s="8"/>
       <c r="E43" s="5"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="C44" s="8"/>
+      <c r="E44" s="5"/>
+      <c r="G44" s="6"/>
+    </row>
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1797,12 +1841,7 @@
     <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="C63" s="8"/>
-      <c r="E63" s="5"/>
-      <c r="G63" s="6"/>
-    </row>
+    <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="C64" s="8"/>
@@ -7431,6 +7470,12 @@
       <c r="E1001" s="5"/>
       <c r="G1001" s="6"/>
     </row>
+    <row r="1002" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1002" s="7"/>
+      <c r="C1002" s="8"/>
+      <c r="E1002" s="5"/>
+      <c r="G1002" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>